<commit_message>
fiducial=False, %sys_c -> %norm_c
</commit_message>
<xml_diff>
--- a/dy_qT/expdata/90001.xlsx
+++ b/dy_qT/expdata/90001.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avp5627/GIT/fitpack2/database/dy_qT/expdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barryp/work/JAM/fitpack2/database/dy_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F2F15F87-087C-CA4B-BAF1-87F0AD395499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96484AF6-EEDE-6F4E-8AF6-53C0E7EEA981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1020" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="860" yWindow="1020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDF1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -90,9 +79,6 @@
     <t>stat_u</t>
   </si>
   <si>
-    <t>%sys_c</t>
-  </si>
-  <si>
     <t>obs</t>
   </si>
   <si>
@@ -122,11 +108,14 @@
   <si>
     <t>pbar</t>
   </si>
+  <si>
+    <t>%norm_c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -961,12 +950,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13:X51"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1008,7 +995,7 @@
         <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="N1" t="s">
         <v>0</v>
@@ -1029,19 +1016,19 @@
         <v>15</v>
       </c>
       <c r="T1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
-      </c>
-      <c r="X1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -1060,11 +1047,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>-1000</v>
-      </c>
-      <c r="G2">
-        <v>1000</v>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0.25</v>
@@ -1093,29 +1080,29 @@
       <c r="P2">
         <v>0</v>
       </c>
-      <c r="Q2">
-        <v>-1000</v>
-      </c>
-      <c r="R2">
-        <v>1000</v>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
       </c>
       <c r="S2" t="s">
         <v>17</v>
       </c>
       <c r="T2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
@@ -1134,11 +1121,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>-1000</v>
-      </c>
-      <c r="G3">
-        <v>1000</v>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0.75</v>
@@ -1167,29 +1154,29 @@
       <c r="P3">
         <v>0</v>
       </c>
-      <c r="Q3">
-        <v>-1000</v>
-      </c>
-      <c r="R3">
-        <v>1000</v>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
       </c>
       <c r="S3" t="s">
         <v>17</v>
       </c>
       <c r="T3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1208,11 +1195,11 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>-1000</v>
-      </c>
-      <c r="G4">
-        <v>1000</v>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
       </c>
       <c r="H4">
         <v>1.25</v>
@@ -1241,29 +1228,29 @@
       <c r="P4">
         <v>0</v>
       </c>
-      <c r="Q4">
-        <v>-1000</v>
-      </c>
-      <c r="R4">
-        <v>1000</v>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
       </c>
       <c r="S4" t="s">
         <v>17</v>
       </c>
       <c r="T4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1282,11 +1269,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>-1000</v>
-      </c>
-      <c r="G5">
-        <v>1000</v>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
       </c>
       <c r="H5">
         <v>1.75</v>
@@ -1315,29 +1302,29 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5">
-        <v>-1000</v>
-      </c>
-      <c r="R5">
-        <v>1000</v>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
       </c>
       <c r="S5" t="s">
         <v>17</v>
       </c>
       <c r="T5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -1356,11 +1343,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>-1000</v>
-      </c>
-      <c r="G6">
-        <v>1000</v>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
       </c>
       <c r="H6">
         <v>2.25</v>
@@ -1389,29 +1376,29 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6">
-        <v>-1000</v>
-      </c>
-      <c r="R6">
-        <v>1000</v>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
       </c>
       <c r="S6" t="s">
         <v>17</v>
       </c>
       <c r="T6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
@@ -1430,11 +1417,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>-1000</v>
-      </c>
-      <c r="G7">
-        <v>1000</v>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
       </c>
       <c r="H7">
         <v>2.75</v>
@@ -1463,29 +1450,29 @@
       <c r="P7">
         <v>0</v>
       </c>
-      <c r="Q7">
-        <v>-1000</v>
-      </c>
-      <c r="R7">
-        <v>1000</v>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
       </c>
       <c r="S7" t="s">
         <v>17</v>
       </c>
       <c r="T7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -1504,11 +1491,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>-1000</v>
-      </c>
-      <c r="G8">
-        <v>1000</v>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
       </c>
       <c r="H8">
         <v>3.25</v>
@@ -1537,29 +1524,29 @@
       <c r="P8">
         <v>0</v>
       </c>
-      <c r="Q8">
-        <v>-1000</v>
-      </c>
-      <c r="R8">
-        <v>1000</v>
+      <c r="Q8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
       </c>
       <c r="S8" t="s">
         <v>17</v>
       </c>
       <c r="T8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
@@ -1578,11 +1565,11 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>-1000</v>
-      </c>
-      <c r="G9">
-        <v>1000</v>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
       <c r="H9">
         <v>3.75</v>
@@ -1611,29 +1598,29 @@
       <c r="P9">
         <v>0</v>
       </c>
-      <c r="Q9">
-        <v>-1000</v>
-      </c>
-      <c r="R9">
-        <v>1000</v>
+      <c r="Q9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
       </c>
       <c r="S9" t="s">
         <v>17</v>
       </c>
       <c r="T9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
@@ -1652,11 +1639,11 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>-1000</v>
-      </c>
-      <c r="G10">
-        <v>1000</v>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
       </c>
       <c r="H10">
         <v>4.25</v>
@@ -1685,29 +1672,29 @@
       <c r="P10">
         <v>0</v>
       </c>
-      <c r="Q10">
-        <v>-1000</v>
-      </c>
-      <c r="R10">
-        <v>1000</v>
+      <c r="Q10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" t="b">
+        <v>0</v>
       </c>
       <c r="S10" t="s">
         <v>17</v>
       </c>
       <c r="T10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -1726,11 +1713,11 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>-1000</v>
-      </c>
-      <c r="G11">
-        <v>1000</v>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
       </c>
       <c r="H11">
         <v>4.75</v>
@@ -1759,29 +1746,29 @@
       <c r="P11">
         <v>0</v>
       </c>
-      <c r="Q11">
-        <v>-1000</v>
-      </c>
-      <c r="R11">
-        <v>1000</v>
+      <c r="Q11" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" t="b">
+        <v>0</v>
       </c>
       <c r="S11" t="s">
         <v>17</v>
       </c>
       <c r="T11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1800,11 +1787,11 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>-1000</v>
-      </c>
-      <c r="G12">
-        <v>1000</v>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
       </c>
       <c r="H12">
         <v>5.25</v>
@@ -1833,29 +1820,29 @@
       <c r="P12">
         <v>0</v>
       </c>
-      <c r="Q12">
-        <v>-1000</v>
-      </c>
-      <c r="R12">
-        <v>1000</v>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
       </c>
       <c r="S12" t="s">
         <v>17</v>
       </c>
       <c r="T12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -1874,11 +1861,11 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13">
-        <v>-1000</v>
-      </c>
-      <c r="G13">
-        <v>1000</v>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
       </c>
       <c r="H13">
         <v>5.75</v>
@@ -1907,29 +1894,29 @@
       <c r="P13">
         <v>0</v>
       </c>
-      <c r="Q13">
-        <v>-1000</v>
-      </c>
-      <c r="R13">
-        <v>1000</v>
+      <c r="Q13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" t="b">
+        <v>0</v>
       </c>
       <c r="S13" t="s">
         <v>17</v>
       </c>
       <c r="T13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
@@ -1948,11 +1935,11 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
-        <v>-1000</v>
-      </c>
-      <c r="G14">
-        <v>1000</v>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
       </c>
       <c r="H14">
         <v>6.25</v>
@@ -1981,29 +1968,29 @@
       <c r="P14">
         <v>0</v>
       </c>
-      <c r="Q14">
-        <v>-1000</v>
-      </c>
-      <c r="R14">
-        <v>1000</v>
+      <c r="Q14" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" t="b">
+        <v>0</v>
       </c>
       <c r="S14" t="s">
         <v>17</v>
       </c>
       <c r="T14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -2022,11 +2009,11 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
-        <v>-1000</v>
-      </c>
-      <c r="G15">
-        <v>1000</v>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
       </c>
       <c r="H15">
         <v>6.75</v>
@@ -2055,29 +2042,29 @@
       <c r="P15">
         <v>0</v>
       </c>
-      <c r="Q15">
-        <v>-1000</v>
-      </c>
-      <c r="R15">
-        <v>1000</v>
+      <c r="Q15" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" t="b">
+        <v>0</v>
       </c>
       <c r="S15" t="s">
         <v>17</v>
       </c>
       <c r="T15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
@@ -2096,11 +2083,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
-        <v>-1000</v>
-      </c>
-      <c r="G16">
-        <v>1000</v>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
       </c>
       <c r="H16">
         <v>7.25</v>
@@ -2129,29 +2116,29 @@
       <c r="P16">
         <v>0</v>
       </c>
-      <c r="Q16">
-        <v>-1000</v>
-      </c>
-      <c r="R16">
-        <v>1000</v>
+      <c r="Q16" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" t="b">
+        <v>0</v>
       </c>
       <c r="S16" t="s">
         <v>17</v>
       </c>
       <c r="T16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -2170,11 +2157,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
-        <v>-1000</v>
-      </c>
-      <c r="G17">
-        <v>1000</v>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
       </c>
       <c r="H17">
         <v>7.75</v>
@@ -2203,29 +2190,29 @@
       <c r="P17">
         <v>0</v>
       </c>
-      <c r="Q17">
-        <v>-1000</v>
-      </c>
-      <c r="R17">
-        <v>1000</v>
+      <c r="Q17" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" t="b">
+        <v>0</v>
       </c>
       <c r="S17" t="s">
         <v>17</v>
       </c>
       <c r="T17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
@@ -2244,11 +2231,11 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>-1000</v>
-      </c>
-      <c r="G18">
-        <v>1000</v>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
       </c>
       <c r="H18">
         <v>8.25</v>
@@ -2277,29 +2264,29 @@
       <c r="P18">
         <v>0</v>
       </c>
-      <c r="Q18">
-        <v>-1000</v>
-      </c>
-      <c r="R18">
-        <v>1000</v>
+      <c r="Q18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" t="b">
+        <v>0</v>
       </c>
       <c r="S18" t="s">
         <v>17</v>
       </c>
       <c r="T18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -2318,11 +2305,11 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19">
-        <v>-1000</v>
-      </c>
-      <c r="G19">
-        <v>1000</v>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
       </c>
       <c r="H19">
         <v>8.75</v>
@@ -2351,29 +2338,29 @@
       <c r="P19">
         <v>0</v>
       </c>
-      <c r="Q19">
-        <v>-1000</v>
-      </c>
-      <c r="R19">
-        <v>1000</v>
+      <c r="Q19" t="b">
+        <v>0</v>
+      </c>
+      <c r="R19" t="b">
+        <v>0</v>
       </c>
       <c r="S19" t="s">
         <v>17</v>
       </c>
       <c r="T19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -2392,11 +2379,11 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20">
-        <v>-1000</v>
-      </c>
-      <c r="G20">
-        <v>1000</v>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
       </c>
       <c r="H20">
         <v>9.25</v>
@@ -2425,29 +2412,29 @@
       <c r="P20">
         <v>0</v>
       </c>
-      <c r="Q20">
-        <v>-1000</v>
-      </c>
-      <c r="R20">
-        <v>1000</v>
+      <c r="Q20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" t="b">
+        <v>0</v>
       </c>
       <c r="S20" t="s">
         <v>17</v>
       </c>
       <c r="T20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -2466,11 +2453,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
-        <v>-1000</v>
-      </c>
-      <c r="G21">
-        <v>1000</v>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
       </c>
       <c r="H21">
         <v>9.75</v>
@@ -2499,29 +2486,29 @@
       <c r="P21">
         <v>0</v>
       </c>
-      <c r="Q21">
-        <v>-1000</v>
-      </c>
-      <c r="R21">
-        <v>1000</v>
+      <c r="Q21" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" t="b">
+        <v>0</v>
       </c>
       <c r="S21" t="s">
         <v>17</v>
       </c>
       <c r="T21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -2540,11 +2527,11 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
-        <v>-1000</v>
-      </c>
-      <c r="G22">
-        <v>1000</v>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
       </c>
       <c r="H22">
         <v>10.25</v>
@@ -2573,29 +2560,29 @@
       <c r="P22">
         <v>0</v>
       </c>
-      <c r="Q22">
-        <v>-1000</v>
-      </c>
-      <c r="R22">
-        <v>1000</v>
+      <c r="Q22" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" t="b">
+        <v>0</v>
       </c>
       <c r="S22" t="s">
         <v>17</v>
       </c>
       <c r="T22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
@@ -2614,11 +2601,11 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23">
-        <v>-1000</v>
-      </c>
-      <c r="G23">
-        <v>1000</v>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
       </c>
       <c r="H23">
         <v>10.75</v>
@@ -2647,29 +2634,29 @@
       <c r="P23">
         <v>0</v>
       </c>
-      <c r="Q23">
-        <v>-1000</v>
-      </c>
-      <c r="R23">
-        <v>1000</v>
+      <c r="Q23" t="b">
+        <v>0</v>
+      </c>
+      <c r="R23" t="b">
+        <v>0</v>
       </c>
       <c r="S23" t="s">
         <v>17</v>
       </c>
       <c r="T23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2688,11 +2675,11 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24">
-        <v>-1000</v>
-      </c>
-      <c r="G24">
-        <v>1000</v>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
       </c>
       <c r="H24">
         <v>11.25</v>
@@ -2721,29 +2708,29 @@
       <c r="P24">
         <v>0</v>
       </c>
-      <c r="Q24">
-        <v>-1000</v>
-      </c>
-      <c r="R24">
-        <v>1000</v>
+      <c r="Q24" t="b">
+        <v>0</v>
+      </c>
+      <c r="R24" t="b">
+        <v>0</v>
       </c>
       <c r="S24" t="s">
         <v>17</v>
       </c>
       <c r="T24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
@@ -2762,11 +2749,11 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25">
-        <v>-1000</v>
-      </c>
-      <c r="G25">
-        <v>1000</v>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
       </c>
       <c r="H25">
         <v>11.75</v>
@@ -2795,29 +2782,29 @@
       <c r="P25">
         <v>0</v>
       </c>
-      <c r="Q25">
-        <v>-1000</v>
-      </c>
-      <c r="R25">
-        <v>1000</v>
+      <c r="Q25" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" t="b">
+        <v>0</v>
       </c>
       <c r="S25" t="s">
         <v>17</v>
       </c>
       <c r="T25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
@@ -2836,11 +2823,11 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26">
-        <v>-1000</v>
-      </c>
-      <c r="G26">
-        <v>1000</v>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
       </c>
       <c r="H26">
         <v>12.5</v>
@@ -2869,29 +2856,29 @@
       <c r="P26">
         <v>0</v>
       </c>
-      <c r="Q26">
-        <v>-1000</v>
-      </c>
-      <c r="R26">
-        <v>1000</v>
+      <c r="Q26" t="b">
+        <v>0</v>
+      </c>
+      <c r="R26" t="b">
+        <v>0</v>
       </c>
       <c r="S26" t="s">
         <v>17</v>
       </c>
       <c r="T26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
@@ -2910,11 +2897,11 @@
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27">
-        <v>-1000</v>
-      </c>
-      <c r="G27">
-        <v>1000</v>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
       </c>
       <c r="H27">
         <v>13.5</v>
@@ -2943,29 +2930,29 @@
       <c r="P27">
         <v>0</v>
       </c>
-      <c r="Q27">
-        <v>-1000</v>
-      </c>
-      <c r="R27">
-        <v>1000</v>
+      <c r="Q27" t="b">
+        <v>0</v>
+      </c>
+      <c r="R27" t="b">
+        <v>0</v>
       </c>
       <c r="S27" t="s">
         <v>17</v>
       </c>
       <c r="T27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
@@ -2984,11 +2971,11 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28">
-        <v>-1000</v>
-      </c>
-      <c r="G28">
-        <v>1000</v>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
       </c>
       <c r="H28">
         <v>14.5</v>
@@ -3017,29 +3004,29 @@
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="Q28">
-        <v>-1000</v>
-      </c>
-      <c r="R28">
-        <v>1000</v>
+      <c r="Q28" t="b">
+        <v>0</v>
+      </c>
+      <c r="R28" t="b">
+        <v>0</v>
       </c>
       <c r="S28" t="s">
         <v>17</v>
       </c>
       <c r="T28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
@@ -3058,11 +3045,11 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
-        <v>-1000</v>
-      </c>
-      <c r="G29">
-        <v>1000</v>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
       </c>
       <c r="H29">
         <v>15.5</v>
@@ -3091,29 +3078,29 @@
       <c r="P29">
         <v>0</v>
       </c>
-      <c r="Q29">
-        <v>-1000</v>
-      </c>
-      <c r="R29">
-        <v>1000</v>
+      <c r="Q29" t="b">
+        <v>0</v>
+      </c>
+      <c r="R29" t="b">
+        <v>0</v>
       </c>
       <c r="S29" t="s">
         <v>17</v>
       </c>
       <c r="T29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
@@ -3132,11 +3119,11 @@
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30">
-        <v>-1000</v>
-      </c>
-      <c r="G30">
-        <v>1000</v>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
       </c>
       <c r="H30">
         <v>16.5</v>
@@ -3165,29 +3152,29 @@
       <c r="P30">
         <v>0</v>
       </c>
-      <c r="Q30">
-        <v>-1000</v>
-      </c>
-      <c r="R30">
-        <v>1000</v>
+      <c r="Q30" t="b">
+        <v>0</v>
+      </c>
+      <c r="R30" t="b">
+        <v>0</v>
       </c>
       <c r="S30" t="s">
         <v>17</v>
       </c>
       <c r="T30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
@@ -3206,11 +3193,11 @@
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31">
-        <v>-1000</v>
-      </c>
-      <c r="G31">
-        <v>1000</v>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
       </c>
       <c r="H31">
         <v>17.5</v>
@@ -3239,29 +3226,29 @@
       <c r="P31">
         <v>0</v>
       </c>
-      <c r="Q31">
-        <v>-1000</v>
-      </c>
-      <c r="R31">
-        <v>1000</v>
+      <c r="Q31" t="b">
+        <v>0</v>
+      </c>
+      <c r="R31" t="b">
+        <v>0</v>
       </c>
       <c r="S31" t="s">
         <v>17</v>
       </c>
       <c r="T31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
@@ -3280,11 +3267,11 @@
       <c r="E32">
         <v>0</v>
       </c>
-      <c r="F32">
-        <v>-1000</v>
-      </c>
-      <c r="G32">
-        <v>1000</v>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
       </c>
       <c r="H32">
         <v>18.5</v>
@@ -3313,29 +3300,29 @@
       <c r="P32">
         <v>0</v>
       </c>
-      <c r="Q32">
-        <v>-1000</v>
-      </c>
-      <c r="R32">
-        <v>1000</v>
+      <c r="Q32" t="b">
+        <v>0</v>
+      </c>
+      <c r="R32" t="b">
+        <v>0</v>
       </c>
       <c r="S32" t="s">
         <v>17</v>
       </c>
       <c r="T32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
@@ -3354,11 +3341,11 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33">
-        <v>-1000</v>
-      </c>
-      <c r="G33">
-        <v>1000</v>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
       </c>
       <c r="H33">
         <v>19.5</v>
@@ -3387,29 +3374,29 @@
       <c r="P33">
         <v>0</v>
       </c>
-      <c r="Q33">
-        <v>-1000</v>
-      </c>
-      <c r="R33">
-        <v>1000</v>
+      <c r="Q33" t="b">
+        <v>0</v>
+      </c>
+      <c r="R33" t="b">
+        <v>0</v>
       </c>
       <c r="S33" t="s">
         <v>17</v>
       </c>
       <c r="T33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
@@ -3428,11 +3415,11 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34">
-        <v>-1000</v>
-      </c>
-      <c r="G34">
-        <v>1000</v>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
       </c>
       <c r="H34">
         <v>21</v>
@@ -3461,29 +3448,29 @@
       <c r="P34">
         <v>0</v>
       </c>
-      <c r="Q34">
-        <v>-1000</v>
-      </c>
-      <c r="R34">
-        <v>1000</v>
+      <c r="Q34" t="b">
+        <v>0</v>
+      </c>
+      <c r="R34" t="b">
+        <v>0</v>
       </c>
       <c r="S34" t="s">
         <v>17</v>
       </c>
       <c r="T34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
@@ -3502,11 +3489,11 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35">
-        <v>-1000</v>
-      </c>
-      <c r="G35">
-        <v>1000</v>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
       </c>
       <c r="H35">
         <v>23</v>
@@ -3535,29 +3522,29 @@
       <c r="P35">
         <v>0</v>
       </c>
-      <c r="Q35">
-        <v>-1000</v>
-      </c>
-      <c r="R35">
-        <v>1000</v>
+      <c r="Q35" t="b">
+        <v>0</v>
+      </c>
+      <c r="R35" t="b">
+        <v>0</v>
       </c>
       <c r="S35" t="s">
         <v>17</v>
       </c>
       <c r="T35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
@@ -3576,11 +3563,11 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
-        <v>-1000</v>
-      </c>
-      <c r="G36">
-        <v>1000</v>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
       </c>
       <c r="H36">
         <v>25</v>
@@ -3609,29 +3596,29 @@
       <c r="P36">
         <v>0</v>
       </c>
-      <c r="Q36">
-        <v>-1000</v>
-      </c>
-      <c r="R36">
-        <v>1000</v>
+      <c r="Q36" t="b">
+        <v>0</v>
+      </c>
+      <c r="R36" t="b">
+        <v>0</v>
       </c>
       <c r="S36" t="s">
         <v>17</v>
       </c>
       <c r="T36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
@@ -3650,11 +3637,11 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>-1000</v>
-      </c>
-      <c r="G37">
-        <v>1000</v>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
       </c>
       <c r="H37">
         <v>27</v>
@@ -3683,29 +3670,29 @@
       <c r="P37">
         <v>0</v>
       </c>
-      <c r="Q37">
-        <v>-1000</v>
-      </c>
-      <c r="R37">
-        <v>1000</v>
+      <c r="Q37" t="b">
+        <v>0</v>
+      </c>
+      <c r="R37" t="b">
+        <v>0</v>
       </c>
       <c r="S37" t="s">
         <v>17</v>
       </c>
       <c r="T37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
@@ -3724,11 +3711,11 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
-        <v>-1000</v>
-      </c>
-      <c r="G38">
-        <v>1000</v>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
       </c>
       <c r="H38">
         <v>29</v>
@@ -3757,29 +3744,29 @@
       <c r="P38">
         <v>0</v>
       </c>
-      <c r="Q38">
-        <v>-1000</v>
-      </c>
-      <c r="R38">
-        <v>1000</v>
+      <c r="Q38" t="b">
+        <v>0</v>
+      </c>
+      <c r="R38" t="b">
+        <v>0</v>
       </c>
       <c r="S38" t="s">
         <v>17</v>
       </c>
       <c r="T38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
@@ -3798,11 +3785,11 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>-1000</v>
-      </c>
-      <c r="G39">
-        <v>1000</v>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
       </c>
       <c r="H39">
         <v>32</v>
@@ -3831,29 +3818,29 @@
       <c r="P39">
         <v>0</v>
       </c>
-      <c r="Q39">
-        <v>-1000</v>
-      </c>
-      <c r="R39">
-        <v>1000</v>
+      <c r="Q39" t="b">
+        <v>0</v>
+      </c>
+      <c r="R39" t="b">
+        <v>0</v>
       </c>
       <c r="S39" t="s">
         <v>17</v>
       </c>
       <c r="T39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
@@ -3872,11 +3859,11 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>-1000</v>
-      </c>
-      <c r="G40">
-        <v>1000</v>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
       </c>
       <c r="H40">
         <v>36</v>
@@ -3905,29 +3892,29 @@
       <c r="P40">
         <v>0</v>
       </c>
-      <c r="Q40">
-        <v>-1000</v>
-      </c>
-      <c r="R40">
-        <v>1000</v>
+      <c r="Q40" t="b">
+        <v>0</v>
+      </c>
+      <c r="R40" t="b">
+        <v>0</v>
       </c>
       <c r="S40" t="s">
         <v>17</v>
       </c>
       <c r="T40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
@@ -3946,11 +3933,11 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41">
-        <v>-1000</v>
-      </c>
-      <c r="G41">
-        <v>1000</v>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
       </c>
       <c r="H41">
         <v>40</v>
@@ -3979,29 +3966,29 @@
       <c r="P41">
         <v>0</v>
       </c>
-      <c r="Q41">
-        <v>-1000</v>
-      </c>
-      <c r="R41">
-        <v>1000</v>
+      <c r="Q41" t="b">
+        <v>0</v>
+      </c>
+      <c r="R41" t="b">
+        <v>0</v>
       </c>
       <c r="S41" t="s">
         <v>17</v>
       </c>
       <c r="T41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
@@ -4020,11 +4007,11 @@
       <c r="E42">
         <v>0</v>
       </c>
-      <c r="F42">
-        <v>-1000</v>
-      </c>
-      <c r="G42">
-        <v>1000</v>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
       </c>
       <c r="H42">
         <v>44</v>
@@ -4053,29 +4040,29 @@
       <c r="P42">
         <v>0</v>
       </c>
-      <c r="Q42">
-        <v>-1000</v>
-      </c>
-      <c r="R42">
-        <v>1000</v>
+      <c r="Q42" t="b">
+        <v>0</v>
+      </c>
+      <c r="R42" t="b">
+        <v>0</v>
       </c>
       <c r="S42" t="s">
         <v>17</v>
       </c>
       <c r="T42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
@@ -4094,11 +4081,11 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
-        <v>-1000</v>
-      </c>
-      <c r="G43">
-        <v>1000</v>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
       </c>
       <c r="H43">
         <v>48</v>
@@ -4127,29 +4114,29 @@
       <c r="P43">
         <v>0</v>
       </c>
-      <c r="Q43">
-        <v>-1000</v>
-      </c>
-      <c r="R43">
-        <v>1000</v>
+      <c r="Q43" t="b">
+        <v>0</v>
+      </c>
+      <c r="R43" t="b">
+        <v>0</v>
       </c>
       <c r="S43" t="s">
         <v>17</v>
       </c>
       <c r="T43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
@@ -4168,11 +4155,11 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
-        <v>-1000</v>
-      </c>
-      <c r="G44">
-        <v>1000</v>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
       </c>
       <c r="H44">
         <v>55</v>
@@ -4201,29 +4188,29 @@
       <c r="P44">
         <v>0</v>
       </c>
-      <c r="Q44">
-        <v>-1000</v>
-      </c>
-      <c r="R44">
-        <v>1000</v>
+      <c r="Q44" t="b">
+        <v>0</v>
+      </c>
+      <c r="R44" t="b">
+        <v>0</v>
       </c>
       <c r="S44" t="s">
         <v>17</v>
       </c>
       <c r="T44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
@@ -4242,11 +4229,11 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45">
-        <v>-1000</v>
-      </c>
-      <c r="G45">
-        <v>1000</v>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
       </c>
       <c r="H45">
         <v>65</v>
@@ -4275,29 +4262,29 @@
       <c r="P45">
         <v>0</v>
       </c>
-      <c r="Q45">
-        <v>-1000</v>
-      </c>
-      <c r="R45">
-        <v>1000</v>
+      <c r="Q45" t="b">
+        <v>0</v>
+      </c>
+      <c r="R45" t="b">
+        <v>0</v>
       </c>
       <c r="S45" t="s">
         <v>17</v>
       </c>
       <c r="T45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
@@ -4316,11 +4303,11 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>-1000</v>
-      </c>
-      <c r="G46">
-        <v>1000</v>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
       </c>
       <c r="H46">
         <v>75</v>
@@ -4349,29 +4336,29 @@
       <c r="P46">
         <v>0</v>
       </c>
-      <c r="Q46">
-        <v>-1000</v>
-      </c>
-      <c r="R46">
-        <v>1000</v>
+      <c r="Q46" t="b">
+        <v>0</v>
+      </c>
+      <c r="R46" t="b">
+        <v>0</v>
       </c>
       <c r="S46" t="s">
         <v>17</v>
       </c>
       <c r="T46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
@@ -4390,11 +4377,11 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
-        <v>-1000</v>
-      </c>
-      <c r="G47">
-        <v>1000</v>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
       </c>
       <c r="H47">
         <v>85</v>
@@ -4423,29 +4410,29 @@
       <c r="P47">
         <v>0</v>
       </c>
-      <c r="Q47">
-        <v>-1000</v>
-      </c>
-      <c r="R47">
-        <v>1000</v>
+      <c r="Q47" t="b">
+        <v>0</v>
+      </c>
+      <c r="R47" t="b">
+        <v>0</v>
       </c>
       <c r="S47" t="s">
         <v>17</v>
       </c>
       <c r="T47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
@@ -4464,11 +4451,11 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>-1000</v>
-      </c>
-      <c r="G48">
-        <v>1000</v>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
       </c>
       <c r="H48">
         <v>95</v>
@@ -4497,29 +4484,29 @@
       <c r="P48">
         <v>0</v>
       </c>
-      <c r="Q48">
-        <v>-1000</v>
-      </c>
-      <c r="R48">
-        <v>1000</v>
+      <c r="Q48" t="b">
+        <v>0</v>
+      </c>
+      <c r="R48" t="b">
+        <v>0</v>
       </c>
       <c r="S48" t="s">
         <v>17</v>
       </c>
       <c r="T48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
@@ -4538,11 +4525,11 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
-        <v>-1000</v>
-      </c>
-      <c r="G49">
-        <v>1000</v>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
       </c>
       <c r="H49">
         <v>112.5</v>
@@ -4571,29 +4558,29 @@
       <c r="P49">
         <v>0</v>
       </c>
-      <c r="Q49">
-        <v>-1000</v>
-      </c>
-      <c r="R49">
-        <v>1000</v>
+      <c r="Q49" t="b">
+        <v>0</v>
+      </c>
+      <c r="R49" t="b">
+        <v>0</v>
       </c>
       <c r="S49" t="s">
         <v>17</v>
       </c>
       <c r="T49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
@@ -4612,11 +4599,11 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50">
-        <v>-1000</v>
-      </c>
-      <c r="G50">
-        <v>1000</v>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
       </c>
       <c r="H50">
         <v>137.5</v>
@@ -4645,29 +4632,29 @@
       <c r="P50">
         <v>0</v>
       </c>
-      <c r="Q50">
-        <v>-1000</v>
-      </c>
-      <c r="R50">
-        <v>1000</v>
+      <c r="Q50" t="b">
+        <v>0</v>
+      </c>
+      <c r="R50" t="b">
+        <v>0</v>
       </c>
       <c r="S50" t="s">
         <v>17</v>
       </c>
       <c r="T50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
@@ -4686,11 +4673,11 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
-        <v>-1000</v>
-      </c>
-      <c r="G51">
-        <v>1000</v>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
       </c>
       <c r="H51">
         <v>175</v>
@@ -4719,29 +4706,29 @@
       <c r="P51">
         <v>0</v>
       </c>
-      <c r="Q51">
-        <v>-1000</v>
-      </c>
-      <c r="R51">
-        <v>1000</v>
+      <c r="Q51" t="b">
+        <v>0</v>
+      </c>
+      <c r="R51" t="b">
+        <v>0</v>
       </c>
       <c r="S51" t="s">
         <v>17</v>
       </c>
       <c r="T51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove the % in the rows
</commit_message>
<xml_diff>
--- a/dy_qT/expdata/90001.xlsx
+++ b/dy_qT/expdata/90001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barryp/work/JAM/fitpack2/database/dy_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96484AF6-EEDE-6F4E-8AF6-53C0E7EEA981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FCEB6B-112F-D349-AA8D-21DABCF1BE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3340" yWindow="1020" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDF1" sheetId="1" r:id="rId1"/>
@@ -595,7 +595,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -953,9 +953,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -994,7 +999,7 @@
       <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="N1" t="s">
@@ -1069,7 +1074,7 @@
         <v>0.54</v>
       </c>
       <c r="M2" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N2" t="b">
         <v>0</v>
@@ -1143,7 +1148,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N3" t="b">
         <v>0</v>
@@ -1217,7 +1222,7 @@
         <v>1.2</v>
       </c>
       <c r="M4" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N4" t="b">
         <v>0</v>
@@ -1291,7 +1296,7 @@
         <v>1.4</v>
       </c>
       <c r="M5" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N5" t="b">
         <v>0</v>
@@ -1365,7 +1370,7 @@
         <v>1.4</v>
       </c>
       <c r="M6" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N6" t="b">
         <v>0</v>
@@ -1439,7 +1444,7 @@
         <v>1.5</v>
       </c>
       <c r="M7" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N7" t="b">
         <v>0</v>
@@ -1513,7 +1518,7 @@
         <v>1.4</v>
       </c>
       <c r="M8" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N8" t="b">
         <v>0</v>
@@ -1587,7 +1592,7 @@
         <v>1.4</v>
       </c>
       <c r="M9" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N9" t="b">
         <v>0</v>
@@ -1661,7 +1666,7 @@
         <v>1.3</v>
       </c>
       <c r="M10" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N10" t="b">
         <v>0</v>
@@ -1735,7 +1740,7 @@
         <v>1.2</v>
       </c>
       <c r="M11" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N11" t="b">
         <v>0</v>
@@ -1809,7 +1814,7 @@
         <v>1.2</v>
       </c>
       <c r="M12" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N12" t="b">
         <v>0</v>
@@ -1883,7 +1888,7 @@
         <v>1.2</v>
       </c>
       <c r="M13" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N13" t="b">
         <v>0</v>
@@ -1957,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N14" t="b">
         <v>0</v>
@@ -2031,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N15" t="b">
         <v>0</v>
@@ -2105,7 +2110,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N16" t="b">
         <v>0</v>
@@ -2179,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N17" t="b">
         <v>0</v>
@@ -2253,7 +2258,7 @@
         <v>0.9</v>
       </c>
       <c r="M18" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N18" t="b">
         <v>0</v>
@@ -2327,7 +2332,7 @@
         <v>0.9</v>
       </c>
       <c r="M19" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N19" t="b">
         <v>0</v>
@@ -2401,7 +2406,7 @@
         <v>0.9</v>
       </c>
       <c r="M20" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N20" t="b">
         <v>0</v>
@@ -2475,7 +2480,7 @@
         <v>0.82</v>
       </c>
       <c r="M21" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N21" t="b">
         <v>0</v>
@@ -2549,7 +2554,7 @@
         <v>0.76</v>
       </c>
       <c r="M22" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N22" t="b">
         <v>0</v>
@@ -2623,7 +2628,7 @@
         <v>0.74</v>
       </c>
       <c r="M23" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N23" t="b">
         <v>0</v>
@@ -2697,7 +2702,7 @@
         <v>0.76</v>
       </c>
       <c r="M24" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N24" t="b">
         <v>0</v>
@@ -2771,7 +2776,7 @@
         <v>0.72</v>
       </c>
       <c r="M25" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N25" t="b">
         <v>0</v>
@@ -2845,7 +2850,7 @@
         <v>0.53</v>
       </c>
       <c r="M26" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N26" t="b">
         <v>0</v>
@@ -2919,7 +2924,7 @@
         <v>0.47</v>
       </c>
       <c r="M27" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N27" t="b">
         <v>0</v>
@@ -2993,7 +2998,7 @@
         <v>0.41</v>
       </c>
       <c r="M28" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N28" t="b">
         <v>0</v>
@@ -3067,7 +3072,7 @@
         <v>0.44</v>
       </c>
       <c r="M29" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N29" t="b">
         <v>0</v>
@@ -3141,7 +3146,7 @@
         <v>0.4</v>
       </c>
       <c r="M30" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N30" t="b">
         <v>0</v>
@@ -3215,7 +3220,7 @@
         <v>0.39</v>
       </c>
       <c r="M31" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N31" t="b">
         <v>0</v>
@@ -3289,7 +3294,7 @@
         <v>0.35</v>
       </c>
       <c r="M32" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N32" t="b">
         <v>0</v>
@@ -3363,7 +3368,7 @@
         <v>0.33</v>
       </c>
       <c r="M33" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N33" t="b">
         <v>0</v>
@@ -3437,7 +3442,7 @@
         <v>0.22</v>
       </c>
       <c r="M34" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N34" t="b">
         <v>0</v>
@@ -3511,7 +3516,7 @@
         <v>0.18</v>
       </c>
       <c r="M35" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N35" t="b">
         <v>0</v>
@@ -3585,7 +3590,7 @@
         <v>0.18</v>
       </c>
       <c r="M36" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N36" t="b">
         <v>0</v>
@@ -3659,7 +3664,7 @@
         <v>0.17</v>
       </c>
       <c r="M37" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N37" t="b">
         <v>0</v>
@@ -3733,7 +3738,7 @@
         <v>0.16</v>
       </c>
       <c r="M38" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N38" t="b">
         <v>0</v>
@@ -3807,7 +3812,7 @@
         <v>0.1</v>
       </c>
       <c r="M39" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N39" t="b">
         <v>0</v>
@@ -3881,7 +3886,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="M40" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N40" t="b">
         <v>0</v>
@@ -3955,7 +3960,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="M41" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N41" t="b">
         <v>0</v>
@@ -4029,7 +4034,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="M42" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N42" t="b">
         <v>0</v>
@@ -4103,7 +4108,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="M43" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N43" t="b">
         <v>0</v>
@@ -4177,7 +4182,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="M44" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N44" t="b">
         <v>0</v>
@@ -4251,7 +4256,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="M45" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N45" t="b">
         <v>0</v>
@@ -4325,7 +4330,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="M46" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N46" t="b">
         <v>0</v>
@@ -4399,7 +4404,7 @@
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="M47" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N47" t="b">
         <v>0</v>
@@ -4473,7 +4478,7 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="M48" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N48" t="b">
         <v>0</v>
@@ -4547,7 +4552,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="M49" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N49" t="b">
         <v>0</v>
@@ -4621,7 +4626,7 @@
         <v>2.97E-3</v>
       </c>
       <c r="M50" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N50" t="b">
         <v>0</v>
@@ -4695,7 +4700,7 @@
         <v>7.5600000000000005E-4</v>
       </c>
       <c r="M51" s="1">
-        <v>3.9E-2</v>
+        <v>3.9</v>
       </c>
       <c r="N51" t="b">
         <v>0</v>

</xml_diff>